<commit_message>
Formulario Registro de DatosUsuario v1.0
</commit_message>
<xml_diff>
--- a/myappli/src/public/files/Operaciones_Registros.xlsx
+++ b/myappli/src/public/files/Operaciones_Registros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>N</t>
   </si>
@@ -94,58 +94,121 @@
     <t>ESTADO</t>
   </si>
   <si>
+    <t>17:39:38</t>
+  </si>
+  <si>
+    <t>ASD</t>
+  </si>
+  <si>
+    <t>CTA CTE </t>
+  </si>
+  <si>
+    <t>MOVIMIENTO DE EFECTIVO</t>
+  </si>
+  <si>
+    <t>ACTIVOS</t>
+  </si>
+  <si>
+    <t>27-1-2020</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>72378629</t>
+  </si>
+  <si>
+    <t>ARMAMDO HINOJOSA CCAMA</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>VIGENTE</t>
+  </si>
+  <si>
+    <t>17:36:56</t>
+  </si>
+  <si>
+    <t>CAJA CHICA</t>
+  </si>
+  <si>
+    <t>SERVICIOS</t>
+  </si>
+  <si>
+    <t>EGRESOS</t>
+  </si>
+  <si>
+    <t>25-12-2019</t>
+  </si>
+  <si>
+    <t>Factura</t>
+  </si>
+  <si>
+    <t>F001</t>
+  </si>
+  <si>
+    <t>17:32:45</t>
+  </si>
+  <si>
+    <t>VENTAS</t>
+  </si>
+  <si>
+    <t>INGRESOS</t>
+  </si>
+  <si>
+    <t>25-1-2020</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>16:55:31</t>
+  </si>
+  <si>
+    <t>CTAS POR COBRAR2</t>
+  </si>
+  <si>
+    <t>PASIVOS2</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>16:54:32</t>
+  </si>
+  <si>
+    <t>SUCURSLSAPRUEBA</t>
+  </si>
+  <si>
+    <t>Boleta</t>
+  </si>
+  <si>
+    <t>2313</t>
+  </si>
+  <si>
+    <t>15:36:14</t>
+  </si>
+  <si>
+    <t>PRINCIPAL</t>
+  </si>
+  <si>
+    <t>10-1-2020</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
     <t>15:31:48</t>
   </si>
   <si>
-    <t>CTA CTE </t>
-  </si>
-  <si>
-    <t>SERVICIOS</t>
-  </si>
-  <si>
-    <t>EGRESOS</t>
-  </si>
-  <si>
-    <t>10-1-2020</t>
-  </si>
-  <si>
-    <t>Factura</t>
-  </si>
-  <si>
     <t>01</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>72378629</t>
-  </si>
-  <si>
-    <t>ARMAMDO HINOJOSA CCAMA</t>
-  </si>
-  <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>VIGENTE</t>
-  </si>
-  <si>
-    <t>13:52:57</t>
-  </si>
-  <si>
-    <t>VENTAS</t>
-  </si>
-  <si>
-    <t>INGRESOS</t>
-  </si>
-  <si>
-    <t>Boleta</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>PRODUCTO 1</t>
   </si>
 </sst>
 </file>
@@ -221,7 +284,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -341,7 +404,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>202001</v>
@@ -350,55 +413,55 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>22.03</v>
+        <v>8.47</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>3.97</v>
+        <v>1.53</v>
       </c>
       <c r="T7" s="2" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="U7" s="2" t="n">
         <v>0</v>
@@ -407,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="W7" s="2" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="X7" s="2" t="n">
         <v>0</v>
@@ -419,90 +482,505 @@
         <v>0</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>202000</v>
+        <v>202001</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F8" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="3" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="S8" s="3" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="T8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>202001</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>76.27</v>
+      </c>
+      <c r="S9" s="2" t="n">
+        <v>13.73</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="U9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="X9" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>202001</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="3" t="n">
+        <v>84.75</v>
+      </c>
+      <c r="S10" s="3" t="n">
+        <v>15.25</v>
+      </c>
+      <c r="T10" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="U10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="X10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>202001</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="3" t="s">
+      <c r="F11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="I11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="O11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Q8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R8" s="3" t="n">
+      <c r="P11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>389.83</v>
+      </c>
+      <c r="S11" s="2" t="n">
+        <v>70.17</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>460</v>
+      </c>
+      <c r="U11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2" t="n">
+        <v>460</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>202001</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" s="3" t="n">
+      <c r="O12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" s="3" t="n">
+        <v>88.14</v>
+      </c>
+      <c r="S12" s="3" t="n">
+        <v>15.86</v>
+      </c>
+      <c r="T12" s="3" t="n">
+        <v>104</v>
+      </c>
+      <c r="U12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="3" t="n">
+        <v>104</v>
+      </c>
+      <c r="X12" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>202001</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="U8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" s="3" t="n">
-        <v>36</v>
-      </c>
-      <c r="X8" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="3" t="s">
+      <c r="O13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>22.03</v>
+      </c>
+      <c r="S13" s="2" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="T13" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="U13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="X13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>